<commit_message>
added dusky and northerns
</commit_message>
<xml_diff>
--- a/code_testing/VAST_bridging/GOA/2023_hindcast_datasources.xlsx
+++ b/code_testing/VAST_bridging/GOA/2023_hindcast_datasources.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Gadus macrocephalus</t>
   </si>
@@ -87,6 +87,30 @@
   </si>
   <si>
     <t>Sebastes polyspinis</t>
+  </si>
+  <si>
+    <t>dusky rockfish</t>
+  </si>
+  <si>
+    <t>northern rockfish</t>
+  </si>
+  <si>
+    <t>Data_Geostat_Sebastes_variabilis.rds</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1hiaCSmB8vajir228x-Xo1zhfhdLi2ZgV</t>
+  </si>
+  <si>
+    <t>Data_Geostat_Sebastes_polyspinis.RDS</t>
+  </si>
+  <si>
+    <t>year_start</t>
+  </si>
+  <si>
+    <t>year_end</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1YRMhHOb9MMHa_YsKhxhd_1Sck7ehRY2Z</t>
   </si>
 </sst>
 </file>
@@ -404,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -415,10 +439,10 @@
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.453125" customWidth="1"/>
+    <col min="4" max="7" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -435,10 +459,16 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>21720</v>
       </c>
@@ -454,11 +484,17 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>1990</v>
+      </c>
+      <c r="G2">
+        <v>2021</v>
+      </c>
+      <c r="H2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>30060</v>
       </c>
@@ -474,11 +510,17 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>1990</v>
+      </c>
+      <c r="G3">
+        <v>2021</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>310</v>
       </c>
@@ -494,18 +536,66 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1990</v>
+      </c>
+      <c r="G4">
+        <v>2021</v>
+      </c>
+      <c r="H4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>30152</v>
+      </c>
       <c r="B5" t="s">
         <v>19</v>
       </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>1990</v>
+      </c>
+      <c r="G5">
+        <v>2021</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>30420</v>
+      </c>
       <c r="B6" t="s">
         <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>1984</v>
+      </c>
+      <c r="G6">
+        <v>2021</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added testing for differences
</commit_message>
<xml_diff>
--- a/code_testing/VAST_bridging/GOA/2023_hindcast_datasources.xlsx
+++ b/code_testing/VAST_bridging/GOA/2023_hindcast_datasources.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Gadus macrocephalus</t>
   </si>
@@ -111,16 +111,42 @@
   </si>
   <si>
     <t>https://drive.google.com/drive/folders/1YRMhHOb9MMHa_YsKhxhd_1Sck7ehRY2Z</t>
+  </si>
+  <si>
+    <t>Data_ATF2021_1993plus_all data.csv</t>
+  </si>
+  <si>
+    <t>CSV</t>
+  </si>
+  <si>
+    <t>Atheresthes stomias</t>
+  </si>
+  <si>
+    <t>arrowtooth flounder</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1oC3-kAIcyy7-W2joSkJwX66ynXfo_hCc</t>
+  </si>
+  <si>
+    <t>area_units_correct</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,13 +169,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,21 +457,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -465,10 +495,13 @@
         <v>27</v>
       </c>
       <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>21720</v>
       </c>
@@ -490,11 +523,14 @@
       <c r="G2">
         <v>2021</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>30060</v>
       </c>
@@ -516,11 +552,14 @@
       <c r="G3">
         <v>2021</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>310</v>
       </c>
@@ -542,11 +581,14 @@
       <c r="G4">
         <v>2021</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>30152</v>
       </c>
@@ -568,11 +610,14 @@
       <c r="G5">
         <v>2021</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>30420</v>
       </c>
@@ -594,11 +639,47 @@
       <c r="G6">
         <v>2021</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <v>1E-3</v>
+      </c>
+      <c r="I6" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>10110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>1993</v>
+      </c>
+      <c r="G7">
+        <v>2021</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>